<commit_message>
some updates on prepping the fmri stuff.
</commit_message>
<xml_diff>
--- a/experiment/conditions.xlsx
+++ b/experiment/conditions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xpsy1114/Documents/projects/multiple_clocks/multiple_clocks_repo/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F547FC2-F9C9-FC4F-AC00-635D655EE9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D9229E-7874-3D4B-B25B-AE86C776809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1460" windowWidth="22260" windowHeight="16940" xr2:uid="{AD988C73-7F11-1E41-A530-8005EAAECDEA}"/>
+    <workbookView xWindow="13360" yWindow="-21100" windowWidth="22260" windowHeight="16940" xr2:uid="{AD988C73-7F11-1E41-A530-8005EAAECDEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>square</t>
   </si>
@@ -423,10 +424,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA9A912-1DB1-A847-99AE-C7D4C814BFEC}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>4</v>
+      </c>
+      <c r="L1">
+        <v>7</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593FAD8-92CE-E746-B513-326D7B6A09F5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>